<commit_message>
Update Excel file in vaje/010 folder
The Excel file in the specified folder was updated to reflect the latest changes. Ensure that this version is used moving forward for consistency.
</commit_message>
<xml_diff>
--- a/vaje/010. Excel.xlsx
+++ b/vaje/010. Excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28724"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="337" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1FA8342-CF83-4C33-8793-36CE88500A60}"/>
+  <xr:revisionPtr revIDLastSave="361" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5A56AFE-32F6-455E-B504-67865F46B458}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Copy selection.</t>
   </si>
@@ -203,6 +203,24 @@
   </si>
   <si>
     <t>Oblikuj števila v datumsko obliko "dd-mm-yyyy"...</t>
+  </si>
+  <si>
+    <t>Izracunaj 1+1...</t>
+  </si>
+  <si>
+    <t>Izracunaj vsoto dveh stevil v desno celico...</t>
+  </si>
+  <si>
+    <t>Izracunaj ostanek pri deljenju z 2...</t>
+  </si>
+  <si>
+    <t>Ugotovi ali je stevilka liha...</t>
+  </si>
+  <si>
+    <t>Ugotovi ali stevilka ni enaka 10...</t>
+  </si>
+  <si>
+    <t>Ugotovi ali je stevilka vecja od 10</t>
   </si>
   <si>
     <t>Pogojno oblikuj naslednjo tabelo...</t>
@@ -812,10 +830,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A12:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -952,7 +970,55 @@
       </c>
       <c r="F11">
         <f ca="1">TODAY()</f>
-        <v>45748</v>
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>123</v>
+      </c>
+      <c r="C13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -980,436 +1046,436 @@
   <sheetData>
     <row r="1" spans="1:6" ht="29.25">
       <c r="A1" s="7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="7"/>
       <c r="B2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>72</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="7"/>
       <c r="B3">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="C3">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="E3">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="F3">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="7"/>
       <c r="B4">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="F4">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="7"/>
       <c r="B5">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="D5">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="F5">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7"/>
       <c r="B6">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D6">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E6">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="F6">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="7"/>
       <c r="B7">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="D7">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="E7">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="F7">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="7"/>
       <c r="B8">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C8">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="D8">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="F8">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>55</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="7"/>
       <c r="B9">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E9">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="F9">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>87</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="7"/>
       <c r="B10">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>83</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="7"/>
       <c r="B11">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="C11">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="D11">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="E11">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F11">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="7"/>
       <c r="B12">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="C12">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D12">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="E12">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="F12">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>43</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="7"/>
       <c r="B13">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C13">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="D13">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="E13">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="F13">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>51</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="7"/>
       <c r="B14">
         <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <f ca="1">RANDBETWEEN(1,100)</f>
         <v>99</v>
       </c>
-      <c r="C14">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>13</v>
-      </c>
-      <c r="D14">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>75</v>
-      </c>
       <c r="E14">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="F14">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="7"/>
       <c r="B15">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D15">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="E15">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="F15">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="7"/>
       <c r="B16">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>94</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D16">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E16">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F16">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="7"/>
       <c r="B17">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="C17">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D17">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="E17">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="F17">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>32</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="7"/>
       <c r="B18">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="D18">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E18">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F18">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>79</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="7"/>
       <c r="B19">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D19">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="E19">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F19">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>48</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>